<commit_message>
Userstories und Backlog update
Johanna Terp und Constanze Richter
</commit_message>
<xml_diff>
--- a/doc/Backlog/Product-Backlog/Userstories/Userstories.xlsx
+++ b/doc/Backlog/Product-Backlog/Userstories/Userstories.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="555" windowWidth="16215" windowHeight="7365" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="555" windowWidth="16215" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
     <sheet name="Konkretisierung" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Userstories</t>
   </si>
@@ -30,9 +29,6 @@
     <t>Was</t>
   </si>
   <si>
-    <t>Wofür</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -42,39 +38,15 @@
     <t>Herr Müller</t>
   </si>
   <si>
-    <t>Karte der Messhalle</t>
-  </si>
-  <si>
-    <t>Messpunkte visuell darstellen</t>
-  </si>
-  <si>
-    <t>Karte vorhanden, um Messpunkt visuell darstellen zu können</t>
-  </si>
-  <si>
     <t>neuen Messpunkt hinzufügen</t>
   </si>
   <si>
-    <t>an dieser Stelle ist ein Messpunkt hinzufügbar</t>
-  </si>
-  <si>
-    <t>alle Messwerte</t>
-  </si>
-  <si>
     <t>neue Messwerte hinzufügen</t>
   </si>
   <si>
-    <t>alle Messpunkte sind vorhanden um neue Messwerte hinzuzufügen</t>
-  </si>
-  <si>
     <t>Frau Schneider</t>
   </si>
   <si>
-    <t>Messpunkte archivieren</t>
-  </si>
-  <si>
-    <t>Ablegen nicht mehr benötigter Messpunkte</t>
-  </si>
-  <si>
     <t>Messpunkt kann archiviert werden und ist noch nicht archiviert</t>
   </si>
   <si>
@@ -90,43 +62,73 @@
     <t>Herr Leiser</t>
   </si>
   <si>
-    <t>Sortierte Ansicht der Grenzwertüberschreitungen</t>
-  </si>
-  <si>
-    <t>Nachvollziehbarkeit der Messpunkte bezogen auf ihr Datum</t>
-  </si>
-  <si>
     <t>Sortierung der Grenzwertüberschreitungen nach Datum ist möglich</t>
   </si>
   <si>
-    <t>Nachvollziehbarkeit der Messpunkte bezogen auf ihre Uhrzeit</t>
-  </si>
-  <si>
     <t>Sortierung der Grenzwertüberschreitungen nach Uhrzeit ist möglich</t>
   </si>
   <si>
-    <t>Messpunkte filtern können</t>
-  </si>
-  <si>
-    <t>Auswahlmöglichkeit der Messpunkte</t>
-  </si>
-  <si>
-    <t>Messungen können nach Datum gefiltert werden</t>
-  </si>
-  <si>
-    <t>angelegte Daten exportieren</t>
-  </si>
-  <si>
-    <t>für Geschäftsbericht nutzen</t>
-  </si>
-  <si>
     <t>Import nach Word/ Excel für Geschäftsbericht ist möglich</t>
   </si>
   <si>
-    <t>visuelle Darstellung in externen Programmen</t>
-  </si>
-  <si>
     <t>Import nach Word/ Excel für visuelle Darstellung ist möglich</t>
+  </si>
+  <si>
+    <t>Ziel</t>
+  </si>
+  <si>
+    <t>braucht eine Karte der Messhalle</t>
+  </si>
+  <si>
+    <t>um Messpunkte visuell darstellen zu können</t>
+  </si>
+  <si>
+    <t>Ist eine Karte vorhanden, um Messpunkt visuell darstellen zu können</t>
+  </si>
+  <si>
+    <t>möchte einen neuen Messpunkt hinzufügen</t>
+  </si>
+  <si>
+    <t>An dieser Stelle ist ein Messpunkt hinzufügbar</t>
+  </si>
+  <si>
+    <t>möchte zu allen Messpunkten</t>
+  </si>
+  <si>
+    <t>Alle Messpunkte sind vorhanden um neue Messwerte hinzuzufügen</t>
+  </si>
+  <si>
+    <t>möchte Messpunkte archivieren</t>
+  </si>
+  <si>
+    <t>um nicht mehr benötigte Messpunkte abzulegen</t>
+  </si>
+  <si>
+    <t>möchte eine sortierte Ansicht der Grenzwertüberschreitungen</t>
+  </si>
+  <si>
+    <t>um Messpunkte bezogen auf ihr Datum nachzuvollziehen können</t>
+  </si>
+  <si>
+    <t>um Messpunkte bezogen auf ihr Uhrzeit nachzuvollziehen können</t>
+  </si>
+  <si>
+    <t>möchte Messpunkte filtern können</t>
+  </si>
+  <si>
+    <t>um eine Auswahlmöglichkeit der Messpunkte zu bekommen</t>
+  </si>
+  <si>
+    <t>Messungen können nach Datum/ Uhrzeit gefiltert werden</t>
+  </si>
+  <si>
+    <t>möchte angelegte Daten exportieren</t>
+  </si>
+  <si>
+    <t>um sie für einen Geschäftsbericht zu nutzen</t>
+  </si>
+  <si>
+    <t>um sie in externen Programmen visuelle darstellen zu können</t>
   </si>
 </sst>
 </file>
@@ -738,11 +740,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD14"/>
+  <dimension ref="A2:AMJ14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="10.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
@@ -752,7 +756,6 @@
     <col min="8" max="1024" width="10.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
@@ -772,210 +775,210 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H7" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H9" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="H10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H11" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H12" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="H13" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H14" s="1">
         <v>13</v>
@@ -995,7 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>

</xml_diff>